<commit_message>
Added items to BOM. Added footprints to GIT. Finished Capacitor footprint association. Finished LED footprint association.
</commit_message>
<xml_diff>
--- a/hardware/datasheets/BOM_CC1352R1.XLSX
+++ b/hardware/datasheets/BOM_CC1352R1.XLSX
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23901"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23929"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Parker\Desktop\SeniorDesign\sddec21-07\hardware\datasheets\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/033a6759af201263/School/SS 2021/EE 491/Git Repository/sddec21-07/hardware/datasheets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{8E1AE515-D246-44AF-A8E4-23FC90571950}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="10" documentId="8_{8E1AE515-D246-44AF-A8E4-23FC90571950}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{97BF533E-B577-4C72-A900-5BDE036A7BBC}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="13635" yWindow="-15645" windowWidth="18735" windowHeight="10515" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1858,12 +1858,24 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -1878,7 +1890,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -1887,6 +1899,8 @@
     <xf numFmtId="1" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2227,24 +2241,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I138"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="L49" sqref="L49"/>
+    <sheetView tabSelected="1" topLeftCell="C25" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="G38" activeCellId="2" sqref="E38 F38 G38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="12.42578125" customWidth="1"/>
-    <col min="2" max="2" width="11.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.5703125" customWidth="1"/>
-    <col min="4" max="4" width="27.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="53.42578125" customWidth="1"/>
-    <col min="6" max="6" width="35.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="28.7109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.7109375" customWidth="1"/>
+    <col min="1" max="1" width="12.453125" customWidth="1"/>
+    <col min="2" max="2" width="11.453125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="60.90625" customWidth="1"/>
+    <col min="4" max="4" width="27.453125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="44.90625" customWidth="1"/>
+    <col min="6" max="6" width="35.26953125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="28.7265625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.1796875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.7265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A1" s="3" t="s">
         <v>590</v>
       </c>
@@ -2257,7 +2271,7 @@
       <c r="H1" s="2"/>
       <c r="I1" s="2"/>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A2" s="3" t="s">
         <v>0</v>
       </c>
@@ -2270,7 +2284,7 @@
       <c r="H2" s="2"/>
       <c r="I2" s="2"/>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A3" s="3" t="s">
         <v>1</v>
       </c>
@@ -2283,7 +2297,7 @@
       <c r="H3" s="2"/>
       <c r="I3" s="2"/>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A5" s="5" t="s">
         <v>2</v>
       </c>
@@ -2312,7 +2326,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A6" s="4" t="s">
         <v>11</v>
       </c>
@@ -2341,7 +2355,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A7" s="4" t="s">
         <v>18</v>
       </c>
@@ -2370,7 +2384,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A8" s="4" t="s">
         <v>23</v>
       </c>
@@ -2399,7 +2413,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A9" s="4" t="s">
         <v>28</v>
       </c>
@@ -2428,7 +2442,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A10" s="4" t="s">
         <v>33</v>
       </c>
@@ -2457,7 +2471,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A11" s="4" t="s">
         <v>38</v>
       </c>
@@ -2486,7 +2500,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A12" s="4" t="s">
         <v>43</v>
       </c>
@@ -2515,7 +2529,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A13" s="4" t="s">
         <v>43</v>
       </c>
@@ -2544,7 +2558,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A14" s="4" t="s">
         <v>591</v>
       </c>
@@ -2573,7 +2587,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A15" s="4" t="s">
         <v>47</v>
       </c>
@@ -2602,7 +2616,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A16" s="4" t="s">
         <v>52</v>
       </c>
@@ -2631,7 +2645,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A17" s="4" t="s">
         <v>43</v>
       </c>
@@ -2660,7 +2674,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="18" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A18" s="4" t="s">
         <v>596</v>
       </c>
@@ -2689,7 +2703,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A19" s="4" t="s">
         <v>43</v>
       </c>
@@ -2718,7 +2732,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A20" s="4" t="s">
         <v>59</v>
       </c>
@@ -2747,7 +2761,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A21" s="4" t="s">
         <v>64</v>
       </c>
@@ -2776,7 +2790,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A22" s="4" t="s">
         <v>69</v>
       </c>
@@ -2805,7 +2819,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A23" s="4" t="s">
         <v>74</v>
       </c>
@@ -2834,7 +2848,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A24" s="4" t="s">
         <v>79</v>
       </c>
@@ -2863,20 +2877,20 @@
         <v>17</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A25" s="4" t="s">
         <v>84</v>
       </c>
       <c r="B25" s="3">
         <v>1</v>
       </c>
-      <c r="C25" s="4" t="s">
+      <c r="C25" s="8" t="s">
         <v>85</v>
       </c>
       <c r="D25" s="4" t="s">
         <v>86</v>
       </c>
-      <c r="E25" s="4" t="s">
+      <c r="E25" s="8" t="s">
         <v>87</v>
       </c>
       <c r="F25" s="4" t="s">
@@ -2892,7 +2906,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A26" s="4" t="s">
         <v>89</v>
       </c>
@@ -2921,20 +2935,20 @@
         <v>17</v>
       </c>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A27" s="4" t="s">
         <v>95</v>
       </c>
       <c r="B27" s="3">
         <v>7</v>
       </c>
-      <c r="C27" s="4" t="s">
+      <c r="C27" s="8" t="s">
         <v>96</v>
       </c>
       <c r="D27" s="4" t="s">
         <v>97</v>
       </c>
-      <c r="E27" s="4" t="s">
+      <c r="E27" s="8" t="s">
         <v>98</v>
       </c>
       <c r="F27" s="4" t="s">
@@ -2950,20 +2964,20 @@
         <v>17</v>
       </c>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A28" s="4" t="s">
         <v>100</v>
       </c>
       <c r="B28" s="3">
         <v>6</v>
       </c>
-      <c r="C28" s="4" t="s">
+      <c r="C28" s="9" t="s">
         <v>101</v>
       </c>
       <c r="D28" s="4" t="s">
         <v>102</v>
       </c>
-      <c r="E28" s="4" t="s">
+      <c r="E28" s="9" t="s">
         <v>103</v>
       </c>
       <c r="F28" s="4" t="s">
@@ -2979,7 +2993,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A29" s="4" t="s">
         <v>106</v>
       </c>
@@ -3008,7 +3022,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A30" s="4" t="s">
         <v>43</v>
       </c>
@@ -3037,7 +3051,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A31" s="4" t="s">
         <v>112</v>
       </c>
@@ -3066,7 +3080,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A32" s="4" t="s">
         <v>117</v>
       </c>
@@ -3095,7 +3109,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A33" s="4" t="s">
         <v>122</v>
       </c>
@@ -3124,20 +3138,20 @@
         <v>17</v>
       </c>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A34" s="4" t="s">
         <v>127</v>
       </c>
       <c r="B34" s="3">
         <v>1</v>
       </c>
-      <c r="C34" s="4" t="s">
+      <c r="C34" s="9" t="s">
         <v>128</v>
       </c>
       <c r="D34" s="4" t="s">
         <v>129</v>
       </c>
-      <c r="E34" s="4" t="s">
+      <c r="E34" s="9" t="s">
         <v>130</v>
       </c>
       <c r="F34" s="4" t="s">
@@ -3153,7 +3167,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A35" s="4" t="s">
         <v>43</v>
       </c>
@@ -3182,7 +3196,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A36" s="4" t="s">
         <v>133</v>
       </c>
@@ -3211,7 +3225,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A37" s="4" t="s">
         <v>137</v>
       </c>
@@ -3240,7 +3254,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A38" s="4" t="s">
         <v>143</v>
       </c>
@@ -3269,7 +3283,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A39" s="4" t="s">
         <v>147</v>
       </c>
@@ -3298,7 +3312,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A40" s="4" t="s">
         <v>153</v>
       </c>
@@ -3327,7 +3341,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A41" s="4" t="s">
         <v>43</v>
       </c>
@@ -3356,7 +3370,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A42" s="4" t="s">
         <v>158</v>
       </c>
@@ -3385,7 +3399,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A43" s="4" t="s">
         <v>164</v>
       </c>
@@ -3414,7 +3428,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A44" s="4" t="s">
         <v>169</v>
       </c>
@@ -3443,7 +3457,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A45" s="4" t="s">
         <v>173</v>
       </c>
@@ -3472,7 +3486,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A46" s="4" t="s">
         <v>178</v>
       </c>
@@ -3501,7 +3515,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A47" s="4" t="s">
         <v>183</v>
       </c>
@@ -3530,7 +3544,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A48" s="4" t="s">
         <v>188</v>
       </c>
@@ -3559,7 +3573,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A49" s="4" t="s">
         <v>193</v>
       </c>
@@ -3588,7 +3602,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A50" s="4" t="s">
         <v>198</v>
       </c>
@@ -3617,7 +3631,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A51" s="4" t="s">
         <v>203</v>
       </c>
@@ -3646,7 +3660,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A52" s="4" t="s">
         <v>208</v>
       </c>
@@ -3675,7 +3689,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A53" s="4" t="s">
         <v>213</v>
       </c>
@@ -3704,7 +3718,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A54" s="7" t="s">
         <v>603</v>
       </c>
@@ -3733,7 +3747,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="55" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A55" s="4" t="s">
         <v>219</v>
       </c>
@@ -3762,7 +3776,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="56" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A56" s="4" t="s">
         <v>225</v>
       </c>
@@ -3791,7 +3805,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="57" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A57" s="4" t="s">
         <v>230</v>
       </c>
@@ -3820,7 +3834,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="58" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A58" s="4" t="s">
         <v>43</v>
       </c>
@@ -3849,7 +3863,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="59" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A59" s="4" t="s">
         <v>235</v>
       </c>
@@ -3878,7 +3892,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="60" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A60" s="4" t="s">
         <v>240</v>
       </c>
@@ -3907,7 +3921,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="61" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A61" s="4" t="s">
         <v>245</v>
       </c>
@@ -3936,7 +3950,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="62" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A62" s="4" t="s">
         <v>249</v>
       </c>
@@ -3965,7 +3979,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="63" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A63" s="4" t="s">
         <v>253</v>
       </c>
@@ -3994,7 +4008,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="64" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A64" s="4" t="s">
         <v>43</v>
       </c>
@@ -4023,7 +4037,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="65" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A65" s="4" t="s">
         <v>258</v>
       </c>
@@ -4052,7 +4066,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="66" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A66" s="4" t="s">
         <v>263</v>
       </c>
@@ -4081,7 +4095,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="67" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A67" s="4" t="s">
         <v>268</v>
       </c>
@@ -4110,7 +4124,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="68" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A68" s="4" t="s">
         <v>275</v>
       </c>
@@ -4139,7 +4153,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="69" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A69" s="4" t="s">
         <v>280</v>
       </c>
@@ -4168,7 +4182,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="70" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A70" s="4" t="s">
         <v>285</v>
       </c>
@@ -4197,7 +4211,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="71" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A71" s="4" t="s">
         <v>290</v>
       </c>
@@ -4226,7 +4240,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="72" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A72" s="4" t="s">
         <v>295</v>
       </c>
@@ -4255,7 +4269,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="73" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A73" s="4" t="s">
         <v>300</v>
       </c>
@@ -4284,7 +4298,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="74" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A74" s="4" t="s">
         <v>305</v>
       </c>
@@ -4313,7 +4327,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="75" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A75" s="4" t="s">
         <v>43</v>
       </c>
@@ -4342,7 +4356,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="76" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A76" s="4" t="s">
         <v>311</v>
       </c>
@@ -4371,7 +4385,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="77" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A77" s="4" t="s">
         <v>316</v>
       </c>
@@ -4400,7 +4414,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="78" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A78" s="4" t="s">
         <v>321</v>
       </c>
@@ -4429,7 +4443,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="79" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A79" s="4" t="s">
         <v>326</v>
       </c>
@@ -4458,7 +4472,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="80" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A80" s="4" t="s">
         <v>331</v>
       </c>
@@ -4487,7 +4501,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="81" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A81" s="4" t="s">
         <v>336</v>
       </c>
@@ -4516,7 +4530,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="82" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A82" s="4" t="s">
         <v>43</v>
       </c>
@@ -4545,7 +4559,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="83" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A83" s="4" t="s">
         <v>43</v>
       </c>
@@ -4574,7 +4588,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="84" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A84" s="4" t="s">
         <v>343</v>
       </c>
@@ -4603,7 +4617,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="85" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A85" s="4" t="s">
         <v>349</v>
       </c>
@@ -4632,7 +4646,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="86" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A86" s="4" t="s">
         <v>353</v>
       </c>
@@ -4661,7 +4675,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="87" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A87" s="4" t="s">
         <v>358</v>
       </c>
@@ -4690,7 +4704,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="88" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A88" s="4" t="s">
         <v>363</v>
       </c>
@@ -4719,7 +4733,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="89" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A89" s="4" t="s">
         <v>367</v>
       </c>
@@ -4748,7 +4762,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="90" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A90" s="4" t="s">
         <v>372</v>
       </c>
@@ -4777,7 +4791,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="91" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A91" s="4" t="s">
         <v>377</v>
       </c>
@@ -4806,7 +4820,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="92" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A92" s="4" t="s">
         <v>382</v>
       </c>
@@ -4835,7 +4849,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="93" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A93" s="4" t="s">
         <v>386</v>
       </c>
@@ -4864,7 +4878,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="94" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A94" s="4" t="s">
         <v>390</v>
       </c>
@@ -4893,7 +4907,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="95" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A95" s="4" t="s">
         <v>395</v>
       </c>
@@ -4922,7 +4936,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="96" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A96" s="4" t="s">
         <v>400</v>
       </c>
@@ -4951,7 +4965,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="97" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A97" s="4" t="s">
         <v>43</v>
       </c>
@@ -4980,7 +4994,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="98" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A98" s="4" t="s">
         <v>406</v>
       </c>
@@ -5009,7 +5023,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="99" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A99" s="4" t="s">
         <v>43</v>
       </c>
@@ -5038,7 +5052,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="100" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A100" s="4" t="s">
         <v>412</v>
       </c>
@@ -5067,7 +5081,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="101" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A101" s="4" t="s">
         <v>417</v>
       </c>
@@ -5096,7 +5110,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="102" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A102" s="4" t="s">
         <v>422</v>
       </c>
@@ -5125,7 +5139,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="103" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A103" s="4" t="s">
         <v>427</v>
       </c>
@@ -5154,7 +5168,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="104" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A104" s="4" t="s">
         <v>432</v>
       </c>
@@ -5183,7 +5197,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="105" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A105" s="4" t="s">
         <v>437</v>
       </c>
@@ -5212,7 +5226,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="106" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A106" s="4" t="s">
         <v>442</v>
       </c>
@@ -5241,7 +5255,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="107" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A107" s="4" t="s">
         <v>446</v>
       </c>
@@ -5270,7 +5284,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="108" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A108" s="4" t="s">
         <v>43</v>
       </c>
@@ -5299,7 +5313,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="109" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A109" s="4" t="s">
         <v>452</v>
       </c>
@@ -5328,7 +5342,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="110" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A110" s="4" t="s">
         <v>456</v>
       </c>
@@ -5357,7 +5371,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="111" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A111" s="4" t="s">
         <v>462</v>
       </c>
@@ -5386,7 +5400,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="112" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A112" s="4" t="s">
         <v>467</v>
       </c>
@@ -5415,7 +5429,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="113" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A113" s="4" t="s">
         <v>472</v>
       </c>
@@ -5444,7 +5458,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="114" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A114" s="4" t="s">
         <v>477</v>
       </c>
@@ -5473,7 +5487,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="115" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A115" s="4" t="s">
         <v>482</v>
       </c>
@@ -5502,7 +5516,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="116" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A116" s="4" t="s">
         <v>487</v>
       </c>
@@ -5531,7 +5545,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="117" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A117" s="4" t="s">
         <v>492</v>
       </c>
@@ -5560,7 +5574,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="118" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A118" s="4" t="s">
         <v>497</v>
       </c>
@@ -5589,7 +5603,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="119" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A119" s="4" t="s">
         <v>502</v>
       </c>
@@ -5618,7 +5632,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="120" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A120" s="4" t="s">
         <v>506</v>
       </c>
@@ -5647,7 +5661,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="121" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A121" s="4" t="s">
         <v>510</v>
       </c>
@@ -5676,7 +5690,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="122" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A122" s="4" t="s">
         <v>515</v>
       </c>
@@ -5705,7 +5719,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="123" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A123" s="4" t="s">
         <v>519</v>
       </c>
@@ -5734,7 +5748,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="124" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A124" s="4" t="s">
         <v>524</v>
       </c>
@@ -5763,7 +5777,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="125" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A125" s="4" t="s">
         <v>529</v>
       </c>
@@ -5792,7 +5806,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="126" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A126" s="4" t="s">
         <v>534</v>
       </c>
@@ -5821,7 +5835,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="127" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A127" s="4" t="s">
         <v>43</v>
       </c>
@@ -5850,7 +5864,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="128" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A128" s="4" t="s">
         <v>540</v>
       </c>
@@ -5879,7 +5893,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="129" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A129" s="4" t="s">
         <v>545</v>
       </c>
@@ -5908,7 +5922,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="130" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A130" s="4" t="s">
         <v>549</v>
       </c>
@@ -5937,7 +5951,7 @@
         <v>555</v>
       </c>
     </row>
-    <row r="131" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A131" s="4" t="s">
         <v>556</v>
       </c>
@@ -5966,7 +5980,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="132" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A132" s="4" t="s">
         <v>562</v>
       </c>
@@ -5995,7 +6009,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="133" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A133" s="4" t="s">
         <v>568</v>
       </c>
@@ -6024,7 +6038,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="134" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A134" s="4" t="s">
         <v>573</v>
       </c>
@@ -6053,7 +6067,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="135" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A135" s="4" t="s">
         <v>579</v>
       </c>
@@ -6082,7 +6096,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="136" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A136" s="4" t="s">
         <v>43</v>
       </c>
@@ -6111,7 +6125,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="137" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A137" s="4" t="s">
         <v>43</v>
       </c>
@@ -6140,7 +6154,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="138" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A138" s="4" t="s">
         <v>585</v>
       </c>

</xml_diff>

<commit_message>
Added all Capacitors to BOM
</commit_message>
<xml_diff>
--- a/hardware/datasheets/BOM_CC1352R1.XLSX
+++ b/hardware/datasheets/BOM_CC1352R1.XLSX
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/033a6759af201263/School/SS 2021/EE 491/Git Repository/sddec21-07/hardware/datasheets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="10" documentId="8_{8E1AE515-D246-44AF-A8E4-23FC90571950}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{97BF533E-B577-4C72-A900-5BDE036A7BBC}"/>
+  <xr:revisionPtr revIDLastSave="12" documentId="8_{8E1AE515-D246-44AF-A8E4-23FC90571950}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{3096D4B2-3B9B-4052-94C1-84E39A65E5B2}"/>
   <bookViews>
-    <workbookView xWindow="13635" yWindow="-15645" windowWidth="18735" windowHeight="10515" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="14145" yWindow="-15135" windowWidth="18735" windowHeight="10515" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -2241,8 +2241,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I138"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C25" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="G38" activeCellId="2" sqref="E38 F38 G38"/>
+    <sheetView tabSelected="1" topLeftCell="C4" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>

<commit_message>
Completed BOM except unlabled DNM parts, labled in red. Completed footprint association except onboard antenae
</commit_message>
<xml_diff>
--- a/hardware/datasheets/BOM_CC1352R1.XLSX
+++ b/hardware/datasheets/BOM_CC1352R1.XLSX
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/033a6759af201263/School/SS 2021/EE 491/Git Repository/sddec21-07/hardware/datasheets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="12" documentId="8_{8E1AE515-D246-44AF-A8E4-23FC90571950}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{3096D4B2-3B9B-4052-94C1-84E39A65E5B2}"/>
+  <xr:revisionPtr revIDLastSave="22" documentId="8_{8E1AE515-D246-44AF-A8E4-23FC90571950}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{68EA3443-1699-4A4C-A715-2E9BA48ABFEC}"/>
   <bookViews>
-    <workbookView xWindow="14145" yWindow="-15135" windowWidth="18735" windowHeight="10515" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="20295" yWindow="-16020" windowWidth="20520" windowHeight="12945" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -2241,21 +2241,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I138"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C4" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="G14" sqref="G14"/>
+    <sheetView tabSelected="1" topLeftCell="C5" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A63" activePane="bottomLeft" state="frozen"/>
+      <selection activeCell="A5" sqref="A5"/>
+      <selection pane="bottomLeft" activeCell="G76" sqref="G76"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="12.453125" customWidth="1"/>
     <col min="2" max="2" width="11.453125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="60.90625" customWidth="1"/>
+    <col min="3" max="3" width="55" customWidth="1"/>
     <col min="4" max="4" width="27.453125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="44.90625" customWidth="1"/>
+    <col min="5" max="5" width="81.90625" customWidth="1"/>
     <col min="6" max="6" width="35.26953125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="28.7265625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.1796875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.7265625" customWidth="1"/>
+    <col min="8" max="8" width="12.1796875" hidden="1" customWidth="1"/>
+    <col min="9" max="9" width="11.7265625" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
Added KiCad Project for Relay module. Relay Module schematic v1 ready.
</commit_message>
<xml_diff>
--- a/hardware/datasheets/BOM_CC1352R1.XLSX
+++ b/hardware/datasheets/BOM_CC1352R1.XLSX
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24326"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/033a6759af201263/School/SS 2021/EE 491/Git Repository/sddec21-07/hardware/datasheets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="22" documentId="8_{8E1AE515-D246-44AF-A8E4-23FC90571950}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{68EA3443-1699-4A4C-A715-2E9BA48ABFEC}"/>
+  <xr:revisionPtr revIDLastSave="23" documentId="8_{8E1AE515-D246-44AF-A8E4-23FC90571950}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3D5A0D02-B1DD-4D0D-99D1-8B622571D4D3}"/>
   <bookViews>
-    <workbookView xWindow="20295" yWindow="-16020" windowWidth="20520" windowHeight="12945" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="38310" yWindow="-210" windowWidth="16440" windowHeight="28440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -2241,26 +2241,26 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I138"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C5" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A63" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" topLeftCell="D5" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A45" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="A5" sqref="A5"/>
-      <selection pane="bottomLeft" activeCell="G76" sqref="G76"/>
+      <selection pane="bottomLeft" activeCell="E119" sqref="E119"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.453125" customWidth="1"/>
-    <col min="2" max="2" width="11.453125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.42578125" customWidth="1"/>
+    <col min="2" max="2" width="11.42578125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="55" customWidth="1"/>
-    <col min="4" max="4" width="27.453125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="81.90625" customWidth="1"/>
-    <col min="6" max="6" width="35.26953125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="28.7265625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.1796875" hidden="1" customWidth="1"/>
-    <col min="9" max="9" width="11.7265625" hidden="1" customWidth="1"/>
+    <col min="4" max="4" width="27.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="158.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="35.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="28.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.140625" hidden="1" customWidth="1"/>
+    <col min="9" max="9" width="11.7109375" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>590</v>
       </c>
@@ -2273,7 +2273,7 @@
       <c r="H1" s="2"/>
       <c r="I1" s="2"/>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>0</v>
       </c>
@@ -2286,7 +2286,7 @@
       <c r="H2" s="2"/>
       <c r="I2" s="2"/>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>1</v>
       </c>
@@ -2299,7 +2299,7 @@
       <c r="H3" s="2"/>
       <c r="I3" s="2"/>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
         <v>2</v>
       </c>
@@ -2328,7 +2328,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
         <v>11</v>
       </c>
@@ -2357,7 +2357,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
         <v>18</v>
       </c>
@@ -2386,7 +2386,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
         <v>23</v>
       </c>
@@ -2415,7 +2415,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
         <v>28</v>
       </c>
@@ -2444,7 +2444,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
         <v>33</v>
       </c>
@@ -2473,7 +2473,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
         <v>38</v>
       </c>
@@ -2502,7 +2502,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
         <v>43</v>
       </c>
@@ -2531,7 +2531,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
         <v>43</v>
       </c>
@@ -2560,7 +2560,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
         <v>591</v>
       </c>
@@ -2589,7 +2589,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" s="4" t="s">
         <v>47</v>
       </c>
@@ -2618,7 +2618,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="s">
         <v>52</v>
       </c>
@@ -2647,7 +2647,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="s">
         <v>43</v>
       </c>
@@ -2676,7 +2676,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="18" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="4" t="s">
         <v>596</v>
       </c>
@@ -2705,7 +2705,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" s="4" t="s">
         <v>43</v>
       </c>
@@ -2734,7 +2734,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" s="4" t="s">
         <v>59</v>
       </c>
@@ -2763,7 +2763,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" s="4" t="s">
         <v>64</v>
       </c>
@@ -2792,7 +2792,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" s="4" t="s">
         <v>69</v>
       </c>
@@ -2821,7 +2821,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" s="4" t="s">
         <v>74</v>
       </c>
@@ -2850,7 +2850,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" s="4" t="s">
         <v>79</v>
       </c>
@@ -2879,7 +2879,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" s="4" t="s">
         <v>84</v>
       </c>
@@ -2908,7 +2908,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" s="4" t="s">
         <v>89</v>
       </c>
@@ -2937,7 +2937,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27" s="4" t="s">
         <v>95</v>
       </c>
@@ -2966,7 +2966,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28" s="4" t="s">
         <v>100</v>
       </c>
@@ -2995,7 +2995,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29" s="4" t="s">
         <v>106</v>
       </c>
@@ -3024,7 +3024,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A30" s="4" t="s">
         <v>43</v>
       </c>
@@ -3053,7 +3053,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A31" s="4" t="s">
         <v>112</v>
       </c>
@@ -3082,7 +3082,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A32" s="4" t="s">
         <v>117</v>
       </c>
@@ -3111,7 +3111,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A33" s="4" t="s">
         <v>122</v>
       </c>
@@ -3140,7 +3140,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A34" s="4" t="s">
         <v>127</v>
       </c>
@@ -3169,7 +3169,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A35" s="4" t="s">
         <v>43</v>
       </c>
@@ -3198,7 +3198,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A36" s="4" t="s">
         <v>133</v>
       </c>
@@ -3227,7 +3227,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A37" s="4" t="s">
         <v>137</v>
       </c>
@@ -3256,7 +3256,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A38" s="4" t="s">
         <v>143</v>
       </c>
@@ -3285,7 +3285,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A39" s="4" t="s">
         <v>147</v>
       </c>
@@ -3314,7 +3314,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A40" s="4" t="s">
         <v>153</v>
       </c>
@@ -3343,7 +3343,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A41" s="4" t="s">
         <v>43</v>
       </c>
@@ -3372,7 +3372,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A42" s="4" t="s">
         <v>158</v>
       </c>
@@ -3401,7 +3401,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A43" s="4" t="s">
         <v>164</v>
       </c>
@@ -3430,7 +3430,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A44" s="4" t="s">
         <v>169</v>
       </c>
@@ -3459,7 +3459,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A45" s="4" t="s">
         <v>173</v>
       </c>
@@ -3488,7 +3488,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A46" s="4" t="s">
         <v>178</v>
       </c>
@@ -3517,7 +3517,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A47" s="4" t="s">
         <v>183</v>
       </c>
@@ -3546,7 +3546,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A48" s="4" t="s">
         <v>188</v>
       </c>
@@ -3575,7 +3575,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A49" s="4" t="s">
         <v>193</v>
       </c>
@@ -3604,7 +3604,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A50" s="4" t="s">
         <v>198</v>
       </c>
@@ -3633,7 +3633,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A51" s="4" t="s">
         <v>203</v>
       </c>
@@ -3662,7 +3662,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A52" s="4" t="s">
         <v>208</v>
       </c>
@@ -3691,7 +3691,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="53" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A53" s="4" t="s">
         <v>213</v>
       </c>
@@ -3720,7 +3720,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="54" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A54" s="7" t="s">
         <v>603</v>
       </c>
@@ -3749,7 +3749,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="55" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A55" s="4" t="s">
         <v>219</v>
       </c>
@@ -3778,7 +3778,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="56" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A56" s="4" t="s">
         <v>225</v>
       </c>
@@ -3807,7 +3807,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="57" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A57" s="4" t="s">
         <v>230</v>
       </c>
@@ -3836,7 +3836,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="58" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A58" s="4" t="s">
         <v>43</v>
       </c>
@@ -3865,7 +3865,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="59" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A59" s="4" t="s">
         <v>235</v>
       </c>
@@ -3894,7 +3894,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="60" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A60" s="4" t="s">
         <v>240</v>
       </c>
@@ -3923,7 +3923,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="61" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A61" s="4" t="s">
         <v>245</v>
       </c>
@@ -3952,7 +3952,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="62" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A62" s="4" t="s">
         <v>249</v>
       </c>
@@ -3981,7 +3981,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="63" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A63" s="4" t="s">
         <v>253</v>
       </c>
@@ -4010,7 +4010,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="64" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A64" s="4" t="s">
         <v>43</v>
       </c>
@@ -4039,7 +4039,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="65" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A65" s="4" t="s">
         <v>258</v>
       </c>
@@ -4068,7 +4068,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="66" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A66" s="4" t="s">
         <v>263</v>
       </c>
@@ -4097,7 +4097,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="67" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A67" s="4" t="s">
         <v>268</v>
       </c>
@@ -4126,7 +4126,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="68" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A68" s="4" t="s">
         <v>275</v>
       </c>
@@ -4155,7 +4155,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="69" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A69" s="4" t="s">
         <v>280</v>
       </c>
@@ -4184,7 +4184,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="70" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A70" s="4" t="s">
         <v>285</v>
       </c>
@@ -4213,7 +4213,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="71" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A71" s="4" t="s">
         <v>290</v>
       </c>
@@ -4242,7 +4242,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="72" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A72" s="4" t="s">
         <v>295</v>
       </c>
@@ -4271,7 +4271,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="73" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A73" s="4" t="s">
         <v>300</v>
       </c>
@@ -4300,7 +4300,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="74" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A74" s="4" t="s">
         <v>305</v>
       </c>
@@ -4329,7 +4329,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="75" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A75" s="4" t="s">
         <v>43</v>
       </c>
@@ -4358,7 +4358,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="76" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A76" s="4" t="s">
         <v>311</v>
       </c>
@@ -4387,7 +4387,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="77" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A77" s="4" t="s">
         <v>316</v>
       </c>
@@ -4416,7 +4416,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="78" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A78" s="4" t="s">
         <v>321</v>
       </c>
@@ -4445,7 +4445,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="79" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A79" s="4" t="s">
         <v>326</v>
       </c>
@@ -4474,7 +4474,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="80" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A80" s="4" t="s">
         <v>331</v>
       </c>
@@ -4503,7 +4503,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="81" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A81" s="4" t="s">
         <v>336</v>
       </c>
@@ -4532,7 +4532,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="82" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A82" s="4" t="s">
         <v>43</v>
       </c>
@@ -4561,7 +4561,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="83" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A83" s="4" t="s">
         <v>43</v>
       </c>
@@ -4590,7 +4590,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="84" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A84" s="4" t="s">
         <v>343</v>
       </c>
@@ -4619,7 +4619,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="85" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A85" s="4" t="s">
         <v>349</v>
       </c>
@@ -4648,7 +4648,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="86" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A86" s="4" t="s">
         <v>353</v>
       </c>
@@ -4677,7 +4677,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="87" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A87" s="4" t="s">
         <v>358</v>
       </c>
@@ -4706,7 +4706,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="88" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A88" s="4" t="s">
         <v>363</v>
       </c>
@@ -4735,7 +4735,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="89" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A89" s="4" t="s">
         <v>367</v>
       </c>
@@ -4764,7 +4764,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="90" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A90" s="4" t="s">
         <v>372</v>
       </c>
@@ -4793,7 +4793,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="91" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="91" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A91" s="4" t="s">
         <v>377</v>
       </c>
@@ -4822,7 +4822,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="92" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="92" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A92" s="4" t="s">
         <v>382</v>
       </c>
@@ -4851,7 +4851,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="93" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="93" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A93" s="4" t="s">
         <v>386</v>
       </c>
@@ -4880,7 +4880,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="94" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="94" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A94" s="4" t="s">
         <v>390</v>
       </c>
@@ -4909,7 +4909,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="95" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="95" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A95" s="4" t="s">
         <v>395</v>
       </c>
@@ -4938,7 +4938,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="96" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="96" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A96" s="4" t="s">
         <v>400</v>
       </c>
@@ -4967,7 +4967,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="97" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="97" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A97" s="4" t="s">
         <v>43</v>
       </c>
@@ -4996,7 +4996,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="98" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="98" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A98" s="4" t="s">
         <v>406</v>
       </c>
@@ -5025,7 +5025,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="99" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="99" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A99" s="4" t="s">
         <v>43</v>
       </c>
@@ -5054,7 +5054,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="100" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="100" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A100" s="4" t="s">
         <v>412</v>
       </c>
@@ -5083,7 +5083,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="101" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="101" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A101" s="4" t="s">
         <v>417</v>
       </c>
@@ -5112,7 +5112,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="102" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="102" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A102" s="4" t="s">
         <v>422</v>
       </c>
@@ -5141,7 +5141,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="103" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="103" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A103" s="4" t="s">
         <v>427</v>
       </c>
@@ -5170,7 +5170,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="104" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="104" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A104" s="4" t="s">
         <v>432</v>
       </c>
@@ -5199,7 +5199,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="105" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="105" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A105" s="4" t="s">
         <v>437</v>
       </c>
@@ -5228,7 +5228,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="106" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="106" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A106" s="4" t="s">
         <v>442</v>
       </c>
@@ -5257,7 +5257,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="107" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="107" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A107" s="4" t="s">
         <v>446</v>
       </c>
@@ -5286,7 +5286,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="108" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="108" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A108" s="4" t="s">
         <v>43</v>
       </c>
@@ -5315,7 +5315,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="109" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="109" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A109" s="4" t="s">
         <v>452</v>
       </c>
@@ -5344,7 +5344,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="110" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="110" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A110" s="4" t="s">
         <v>456</v>
       </c>
@@ -5373,7 +5373,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="111" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="111" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A111" s="4" t="s">
         <v>462</v>
       </c>
@@ -5402,7 +5402,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="112" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="112" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A112" s="4" t="s">
         <v>467</v>
       </c>
@@ -5431,7 +5431,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="113" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="113" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A113" s="4" t="s">
         <v>472</v>
       </c>
@@ -5460,7 +5460,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="114" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="114" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A114" s="4" t="s">
         <v>477</v>
       </c>
@@ -5489,7 +5489,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="115" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="115" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A115" s="4" t="s">
         <v>482</v>
       </c>
@@ -5518,7 +5518,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="116" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="116" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A116" s="4" t="s">
         <v>487</v>
       </c>
@@ -5547,7 +5547,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="117" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="117" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A117" s="4" t="s">
         <v>492</v>
       </c>
@@ -5576,7 +5576,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="118" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="118" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A118" s="4" t="s">
         <v>497</v>
       </c>
@@ -5605,7 +5605,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="119" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="119" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A119" s="4" t="s">
         <v>502</v>
       </c>
@@ -5634,7 +5634,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="120" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="120" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A120" s="4" t="s">
         <v>506</v>
       </c>
@@ -5663,7 +5663,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="121" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="121" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A121" s="4" t="s">
         <v>510</v>
       </c>
@@ -5692,7 +5692,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="122" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="122" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A122" s="4" t="s">
         <v>515</v>
       </c>
@@ -5721,7 +5721,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="123" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="123" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A123" s="4" t="s">
         <v>519</v>
       </c>
@@ -5750,7 +5750,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="124" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="124" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A124" s="4" t="s">
         <v>524</v>
       </c>
@@ -5779,7 +5779,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="125" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="125" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A125" s="4" t="s">
         <v>529</v>
       </c>
@@ -5808,7 +5808,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="126" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="126" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A126" s="4" t="s">
         <v>534</v>
       </c>
@@ -5837,7 +5837,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="127" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="127" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A127" s="4" t="s">
         <v>43</v>
       </c>
@@ -5866,7 +5866,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="128" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="128" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A128" s="4" t="s">
         <v>540</v>
       </c>
@@ -5895,7 +5895,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="129" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="129" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A129" s="4" t="s">
         <v>545</v>
       </c>
@@ -5924,7 +5924,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="130" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="130" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A130" s="4" t="s">
         <v>549</v>
       </c>
@@ -5953,7 +5953,7 @@
         <v>555</v>
       </c>
     </row>
-    <row r="131" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="131" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A131" s="4" t="s">
         <v>556</v>
       </c>
@@ -5982,7 +5982,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="132" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="132" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A132" s="4" t="s">
         <v>562</v>
       </c>
@@ -6011,7 +6011,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="133" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="133" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A133" s="4" t="s">
         <v>568</v>
       </c>
@@ -6040,7 +6040,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="134" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="134" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A134" s="4" t="s">
         <v>573</v>
       </c>
@@ -6069,7 +6069,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="135" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="135" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A135" s="4" t="s">
         <v>579</v>
       </c>
@@ -6098,7 +6098,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="136" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="136" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A136" s="4" t="s">
         <v>43</v>
       </c>
@@ -6127,7 +6127,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="137" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="137" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A137" s="4" t="s">
         <v>43</v>
       </c>
@@ -6156,7 +6156,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="138" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="138" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A138" s="4" t="s">
         <v>585</v>
       </c>

</xml_diff>